<commit_message>
20250320 Small updates to compare
</commit_message>
<xml_diff>
--- a/GUI + Reviews/202503/CAC Family.xlsx
+++ b/GUI + Reviews/202503/CAC Family.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://euronext-my.sharepoint.com/personal/csonneveld_euronext_com/Documents/Documents/Projects/GUI + Reviews/202503/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{611B88E5-6E58-47A2-B469-19DF79CD0EA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{D45D90B9-9BC0-4E9F-8ED2-CFD5FC053C8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1FCF2881-F457-452C-8458-B7CE4E216A1D}"/>
   <bookViews>
-    <workbookView xWindow="-315" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-29115" yWindow="-16005" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PX1" sheetId="2" r:id="rId1"/>
@@ -1738,8 +1738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5" x14ac:dyDescent="0.15"/>

</xml_diff>